<commit_message>
added model comparison functions - prediction, summaries
</commit_message>
<xml_diff>
--- a/analysis/data/tables/data_sources.xlsx
+++ b/analysis/data/tables/data_sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahurl\Documents\_work\p041_berlin_transport_cov\analysis\data\processed\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahurl\Documents\_work\p024_gfz_berlin-trees\berlin.trees\analysis\data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A0BCA2-41A3-4DDE-AD61-4BC86FA2339C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A79FD7A-95D4-484D-80E2-A4931637D1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{81895198-9C62-4C93-9E35-5B090025889B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{81895198-9C62-4C93-9E35-5B090025889B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -700,21 +700,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C164DAAA-26B7-4D95-AC26-51CB2201F682}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
-    <col min="4" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="9" width="23.109375" customWidth="1"/>
-    <col min="10" max="11" width="27.109375" customWidth="1"/>
-    <col min="12" max="12" width="25.5546875" customWidth="1"/>
+    <col min="1" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="4" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="9" width="23.140625" customWidth="1"/>
+    <col min="10" max="11" width="27.140625" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,7 +755,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -796,7 +796,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -837,7 +837,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="94.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="94.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -878,7 +878,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -917,7 +917,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
@@ -958,7 +958,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -999,7 +999,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>21</v>
       </c>
       <c r="H10" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I10" s="1">
         <v>0</v>
@@ -1116,7 +1116,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
@@ -1157,7 +1157,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="143.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="143.44999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>49</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>50</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>48</v>
       </c>

</xml_diff>